<commit_message>
Update Feeagh AWQMS Maintenance Comments.xlsx
</commit_message>
<xml_diff>
--- a/FeeaghAWQMS updates/Feeagh AWQMS Maintenance Comments.xlsx
+++ b/FeeaghAWQMS updates/Feeagh AWQMS Maintenance Comments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BurishooleLTER-Public\FeeaghAWQMS updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edeeyto\Documents\GitHub\BurishooleLTER-Public\FeeaghAWQMS updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="385">
   <si>
     <t>Comments</t>
   </si>
@@ -1152,6 +1152,33 @@
   </si>
   <si>
     <t xml:space="preserve">Sonde (66803) back in after calibration. </t>
+  </si>
+  <si>
+    <t>Monthly sampling</t>
+  </si>
+  <si>
+    <t>Calibrated sonde, downloaded data</t>
+  </si>
+  <si>
+    <t>MR service visit - logger out for the week</t>
+  </si>
+  <si>
+    <t>Montly sampling and cleaned sensors</t>
+  </si>
+  <si>
+    <t>Logger our - service visit for MR. Underwater PFD out for checks</t>
+  </si>
+  <si>
+    <t>Logger back out, underwater PFD back out, PRT chain reading dodgy until 8/11/2019</t>
+  </si>
+  <si>
+    <t>PRTr eading again OK, but BP Now reading dodgy</t>
+  </si>
+  <si>
+    <t>Circuit board busted. Sent back to MR</t>
+  </si>
+  <si>
+    <t>PRT box out and sent to MR for replacement</t>
   </si>
 </sst>
 </file>
@@ -1473,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B594"/>
+  <dimension ref="A1:B606"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A577" workbookViewId="0">
-      <selection activeCell="K584" sqref="K584"/>
+      <selection activeCell="B606" sqref="B606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6237,6 +6264,102 @@
         <v>24</v>
       </c>
     </row>
+    <row r="595" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A595" s="1">
+        <v>43663</v>
+      </c>
+      <c r="B595" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="596" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A596" s="1">
+        <v>43672</v>
+      </c>
+      <c r="B596" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="597" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A597" s="1">
+        <v>43676</v>
+      </c>
+      <c r="B597" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="598" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A598" s="1">
+        <v>43697</v>
+      </c>
+      <c r="B598" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="599" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A599" s="1">
+        <v>43705</v>
+      </c>
+      <c r="B599" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="600" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A600" s="1">
+        <v>43727</v>
+      </c>
+      <c r="B600" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="601" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A601" s="1">
+        <v>43733</v>
+      </c>
+      <c r="B601" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="602" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A602" s="1">
+        <v>43768</v>
+      </c>
+      <c r="B602" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="603" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A603" s="1">
+        <v>43774</v>
+      </c>
+      <c r="B603" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="604" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A604" s="1">
+        <v>43777</v>
+      </c>
+      <c r="B604" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="605" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A605" s="1">
+        <v>43788</v>
+      </c>
+      <c r="B605" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="606" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A606" s="1">
+        <v>43866</v>
+      </c>
+      <c r="B606" t="s">
+        <v>384</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>